<commit_message>
Proceso edición guía didáctica
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion11/ESCALETA_MA_08_11_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion11/ESCALETA_MA_08_11_CO.xlsx
@@ -1414,6 +1414,36 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1485,36 +1515,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,103 +1841,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="158" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="150" t="s">
+      <c r="B1" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="152" t="s">
+      <c r="C1" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="148" t="s">
+      <c r="D1" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="150" t="s">
+      <c r="E1" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="154" t="s">
+      <c r="F1" s="164" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="156" t="s">
+      <c r="G1" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="154" t="s">
+      <c r="H1" s="164" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="154" t="s">
+      <c r="I1" s="164" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="158" t="s">
+      <c r="J1" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="160" t="s">
+      <c r="K1" s="170" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="146" t="s">
+      <c r="L1" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="168" t="s">
+      <c r="M1" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="168"/>
-      <c r="O1" s="169" t="s">
+      <c r="N1" s="145"/>
+      <c r="O1" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="171" t="s">
+      <c r="P1" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="166" t="s">
+      <c r="Q1" s="143" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="173" t="s">
+      <c r="R1" s="150" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="166" t="s">
+      <c r="S1" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="162" t="s">
+      <c r="T1" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="164" t="s">
+      <c r="U1" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="142" t="s">
+      <c r="V1" s="152" t="s">
         <v>153</v>
       </c>
-      <c r="W1" s="144" t="s">
+      <c r="W1" s="154" t="s">
         <v>154</v>
       </c>
       <c r="X1" s="113"/>
     </row>
     <row r="2" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="149"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="147"/>
+      <c r="A2" s="159"/>
+      <c r="B2" s="161"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="171"/>
+      <c r="L2" s="157"/>
       <c r="M2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="N2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="170"/>
-      <c r="P2" s="172"/>
-      <c r="Q2" s="167"/>
-      <c r="R2" s="174"/>
-      <c r="S2" s="167"/>
-      <c r="T2" s="163"/>
-      <c r="U2" s="165"/>
-      <c r="V2" s="143"/>
-      <c r="W2" s="145"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="144"/>
+      <c r="R2" s="151"/>
+      <c r="S2" s="144"/>
+      <c r="T2" s="173"/>
+      <c r="U2" s="175"/>
+      <c r="V2" s="153"/>
+      <c r="W2" s="155"/>
       <c r="X2" s="114" t="s">
         <v>155</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="F22" s="90" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="175" t="s">
+      <c r="G22" s="142" t="s">
         <v>121</v>
       </c>
       <c r="H22" s="119">
@@ -3223,7 +3223,7 @@
       <c r="F23" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="175" t="s">
+      <c r="G23" s="142" t="s">
         <v>126</v>
       </c>
       <c r="H23" s="119">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="E24" s="68"/>
       <c r="F24" s="90"/>
-      <c r="G24" s="175" t="s">
+      <c r="G24" s="142" t="s">
         <v>129</v>
       </c>
       <c r="H24" s="119">
@@ -3709,12 +3709,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="L1:L2"/>
@@ -3731,6 +3725,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>